<commit_message>
aggiornato stime al 2 agosto
</commit_message>
<xml_diff>
--- a/stime_partiti.xlsx
+++ b/stime_partiti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_vari_miei\dati_simulatore_elettorale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_vari_miei\simulatore\dati_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B73E715-67C0-4683-AD96-F58C8A649212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E17E78-AC7A-48BC-AA18-5E16B9B492D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E24C64F7-9734-40BD-9AC2-A6785A14A1CD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E24C64F7-9734-40BD-9AC2-A6785A14A1CD}"/>
   </bookViews>
   <sheets>
     <sheet name="STIME" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="55">
   <si>
     <t>party</t>
   </si>
@@ -142,9 +142,6 @@
     <t>AZN*IV</t>
   </si>
   <si>
-    <t>PD*LEUV*AZN*IV</t>
-  </si>
-  <si>
     <t>PD*LEUV*M5S</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
     <t>PD si allea con LEUV e  M5S, mentre AZN si allea con IV=  FDI*LEGA*FI &amp; PD*LEUV*M5S &amp; AZN&amp;IV</t>
   </si>
   <si>
-    <t>PD si allea con LEUV, AZN e IV =  FDI*LEGA*FI &amp; PD*LEUV*AZN*IV</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
@@ -172,9 +166,6 @@
     <t>descrizione lunga</t>
   </si>
   <si>
-    <t xml:space="preserve">PD si allea con LEUV, AZN e IV </t>
-  </si>
-  <si>
     <t>IPF</t>
   </si>
   <si>
@@ -197,6 +188,24 @@
   </si>
   <si>
     <t>lightgreen</t>
+  </si>
+  <si>
+    <t>PD*AZN*IPF</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>PD si allea con AZN e IPF</t>
+  </si>
+  <si>
+    <t>PD si allea con  AZN e IPF =  FDI*LEGA*FI &amp; PD*AZN</t>
+  </si>
+  <si>
+    <t>fonte</t>
+  </si>
+  <si>
+    <t>SWG 2 agosto</t>
   </si>
 </sst>
 </file>
@@ -573,112 +582,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78552D5-3AB5-477F-A17B-9F49F54AA4DA}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>0.22800000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3">
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3">
-        <v>0.221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="4">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="3"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <f>1-SUM(B2:B11)</f>
+        <v>4.0000000000000036E-2</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B9" xr:uid="{C78552D5-3AB5-477F-A17B-9F49F54AA4DA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -686,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E61A90B-8F5B-4FD2-AF98-2FFAD459D0AA}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -827,10 +850,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -842,7 +865,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -854,7 +877,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -871,7 +894,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -995,7 +1018,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>32</v>
@@ -1004,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1021,7 +1044,7 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,7 +1055,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -1046,16 +1069,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1063,16 +1086,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
         <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1094,19 +1117,19 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1120,7 +1143,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,13 +1155,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1146,10 +1169,10 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1157,10 +1180,10 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1168,10 +1191,10 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1179,10 +1202,10 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiornamento sistema ripartizione e coalizioni
</commit_message>
<xml_diff>
--- a/stime_partiti.xlsx
+++ b/stime_partiti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_vari_miei\dati_simulatore_elettorale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_vari_miei\simulatore\dati_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3952EBD7-53E8-4371-BA47-4EB5B4E27C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A407AE-263F-4D44-8068-EDB89865C2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E24C64F7-9734-40BD-9AC2-A6785A14A1CD}"/>
+    <workbookView xWindow="768" yWindow="696" windowWidth="13740" windowHeight="9192" firstSheet="2" activeTab="2" xr2:uid="{E24C64F7-9734-40BD-9AC2-A6785A14A1CD}"/>
   </bookViews>
   <sheets>
     <sheet name="STIME" sheetId="1" r:id="rId1"/>
@@ -175,6 +175,9 @@
     <t>fonte</t>
   </si>
   <si>
+    <t>SWG 2 agosto</t>
+  </si>
+  <si>
     <t>SI-VERDI</t>
   </si>
   <si>
@@ -184,9 +187,6 @@
     <t>PD*SI-VERDI*M5S</t>
   </si>
   <si>
-    <t>PD*SI-VERDI</t>
-  </si>
-  <si>
     <t>PD si allea con AZN, IPF e SI-VERDI</t>
   </si>
   <si>
@@ -199,13 +199,13 @@
     <t>PD si allea con SI-VERDI e  M5S, mentre AZN si allea con IV=  FDI*LEGA*FI &amp; PD*SI-VERDI*M5S &amp; AZN&amp;IV</t>
   </si>
   <si>
-    <t xml:space="preserve">PD si allea solo con SI-VERDI </t>
-  </si>
-  <si>
-    <t>PD si allea solo con SI-VERDI =  FDI*LEGA*FI &amp; PD*SI-VERDI</t>
-  </si>
-  <si>
-    <t>SWG 2 agosto 2022</t>
+    <t>PD si con SI-VERDI e IPF</t>
+  </si>
+  <si>
+    <t>PD si allea solo con SI-VERDI e IPF =  FDI*LEGA*FI &amp; PD*SI-VERDI*IPF</t>
+  </si>
+  <si>
+    <t>PD*SI-VERDI*IPF</t>
   </si>
 </sst>
 </file>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C78552D5-3AB5-477F-A17B-9F49F54AA4DA}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,7 +614,7 @@
         <v>0.24199999999999999</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -675,7 +675,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4">
         <v>4.1000000000000002E-2</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -893,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3F13D4-FD38-4AB3-83D8-8540DB632A4F}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,16 +977,16 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="str">
+        <f>B5</f>
+        <v>ITALEX</v>
+      </c>
+      <c r="D5" t="str">
         <f>E5</f>
         <v>ITALEX</v>
-      </c>
-      <c r="C5" t="str">
-        <f>D5</f>
-        <v>ITALEX</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
       </c>
       <c r="E5" t="str">
         <f>C5</f>
@@ -997,16 +997,16 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="str">
+        <f>B6</f>
+        <v>ALTRI</v>
+      </c>
+      <c r="D6" t="str">
         <f>E6</f>
         <v>ALTRI</v>
-      </c>
-      <c r="C6" t="str">
-        <f>D6</f>
-        <v>ALTRI</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" t="str">
         <f>C6</f>
@@ -1018,13 +1018,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>39</v>
@@ -1055,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -1069,13 +1069,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -1083,19 +1083,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1120,13 +1120,13 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
         <v>39</v>
@@ -1143,7 +1143,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1169,10 +1169,10 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1191,10 +1191,10 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>